<commit_message>
phân chia công việc
</commit_message>
<xml_diff>
--- a/Documents/ProductBacklog (Version 0.5).xlsx
+++ b/Documents/ProductBacklog (Version 0.5).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JavaWeb\swp391-onlineshop-gr1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BEAN\Desktop\swp391-onlineshop-gr1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E498C5C-E8A5-4C23-9914-9A6F05FC412A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10545" windowHeight="3660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC (SWP391)</t>
   </si>
@@ -187,7 +188,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -197,7 +198,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -217,9 +218,6 @@
     <t>Products List [Sale]</t>
   </si>
   <si>
-    <t>Orders List [Admin]</t>
-  </si>
-  <si>
     <t>Admin views list of all of orders</t>
   </si>
   <si>
@@ -236,13 +234,49 @@
   </si>
   <si>
     <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Orders List [Sale]</t>
+  </si>
+  <si>
+    <t>Trần Văn Đức</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Mạnh</t>
+  </si>
+  <si>
+    <t>Nguyễn Gia Phú</t>
+  </si>
+  <si>
+    <t>Đinh Tiến Lâm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đinh Tiến Lâm </t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>Tìm hiểu thêm về GMAIL API</t>
+  </si>
+  <si>
+    <t>Bạch Ngọc Minh Châu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEADER + FOOTER + ERROR </t>
+  </si>
+  <si>
+    <t>Ngô Thị Ngọc Mai</t>
+  </si>
+  <si>
+    <t>02/010/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -316,7 +350,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -332,7 +366,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -340,7 +374,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -370,8 +404,61 @@
       <color rgb="FF00B050"/>
       <name val="Sitka Display"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Sitka Display"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,12 +474,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFD9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,6 +516,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -527,13 +626,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,34 +638,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="12" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="12" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -587,46 +683,166 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="28" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="28" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="28" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -982,121 +1198,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="44.125" customWidth="1"/>
-    <col min="5" max="5" width="25.25" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
-    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="44.09765625" customWidth="1"/>
+    <col min="5" max="5" width="25.19921875" customWidth="1"/>
+    <col min="6" max="6" width="18.8984375" customWidth="1"/>
+    <col min="7" max="7" width="22.19921875" customWidth="1"/>
+    <col min="8" max="8" width="16.09765625" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="15" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="16" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:9" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="17"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1121,492 +1337,541 @@
       <c r="H9" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23">
+      <c r="I9" s="74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22">
         <v>1</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
+      <c r="F10" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22">
         <v>2</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
+      <c r="F11" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="56">
         <v>3</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23">
+      <c r="F12" s="35"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43">
         <v>4</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="F13" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43">
         <v>5</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="37" t="s">
+      <c r="E14" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22">
+        <v>6</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
+        <v>7</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="22">
+        <v>8</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22">
+        <v>9</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="22">
+        <v>10</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="22">
+        <v>11</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22">
+        <v>12</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22">
+        <v>13</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22">
+        <v>14</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="22">
+        <v>15</v>
+      </c>
+      <c r="B24" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
-        <v>6</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
-        <v>7</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="30" t="s">
+      <c r="D24" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="22">
+        <v>16</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
-        <v>8</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="30" t="s">
+      <c r="D25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22">
+        <v>17</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
-        <v>9</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="31" t="s">
+      <c r="D26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="64">
+        <v>18</v>
+      </c>
+      <c r="B27" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="64">
+        <v>19</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="23">
+        <v>20</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="22">
+        <v>21</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="49">
+        <v>22</v>
+      </c>
+      <c r="B31" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>10</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
-        <v>11</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
-        <v>12</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
-        <v>13</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23">
-        <v>14</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23">
-        <v>15</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23">
-        <v>16</v>
-      </c>
-      <c r="B25" s="32" t="s">
+      <c r="D31" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23">
-        <v>17</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
-        <v>18</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
-        <v>19</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
-        <v>20</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23">
-        <v>21</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
-        <v>22</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1614,10 +1879,10 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="25"/>
+      <c r="H32" s="24"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1625,10 +1890,10 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="25"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1636,10 +1901,10 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="24"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1647,10 +1912,10 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="25"/>
+      <c r="H35" s="24"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1661,7 +1926,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>

</xml_diff>